<commit_message>
-Updated the IFP Reports -Updated the budget templates
Former-commit-id: c470074551b8e43795c7ef1c5bbd43d71b02c542
</commit_message>
<xml_diff>
--- a/data/TVN - FINAL Report.xlsx
+++ b/data/TVN - FINAL Report.xlsx
@@ -134,7 +134,7 @@
     <t>6) *Materials, supplies &amp; other expenditures</t>
   </si>
   <si>
-    <t>8) *Travel</t>
+    <t>7) *Travel</t>
   </si>
   <si>
     <t>Total Expenditures Incurred</t>
@@ -194,7 +194,7 @@
     <t>[Enter Expense Name]</t>
   </si>
   <si>
-    <t>8) Travel</t>
+    <t>7) Travel</t>
   </si>
   <si>
     <t>No. of Trip</t>
@@ -1536,7 +1536,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal 3" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 3" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1607,10 +1607,10 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4014,7 +4014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="22.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="33" t="s">
         <v>30</v>
       </c>
@@ -4104,6 +4104,8 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="24">
     <mergeCell ref="A1:H1"/>
@@ -4149,8 +4151,8 @@
   </sheetPr>
   <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5357,7 +5359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="79" t="s">
         <v>45</v>
       </c>
@@ -5371,7 +5373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="79" t="s">
         <v>45</v>
       </c>
@@ -5385,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="79" t="s">
         <v>45</v>
       </c>
@@ -5399,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="67" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="74" t="s">
         <v>46</v>
       </c>
@@ -5408,7 +5410,7 @@
       <c r="D16" s="74"/>
       <c r="E16" s="74"/>
     </row>
-    <row r="17" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="78" t="s">
         <v>47</v>
       </c>
@@ -5423,7 +5425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="79" t="s">
         <v>48</v>
       </c>
@@ -5437,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="79" t="s">
         <v>48</v>
       </c>
@@ -5451,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="79" t="s">
         <v>48</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" s="67" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="74" t="s">
         <v>46</v>
       </c>
@@ -5474,7 +5476,7 @@
       <c r="D21" s="74"/>
       <c r="E21" s="74"/>
     </row>
-    <row r="22" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="78" t="s">
         <v>49</v>
       </c>
@@ -5489,7 +5491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="79" t="s">
         <v>50</v>
       </c>
@@ -5503,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="79" t="s">
         <v>50</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="79" t="s">
         <v>50</v>
       </c>
@@ -5531,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" s="67" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="74" t="s">
         <v>46</v>
       </c>
@@ -5540,7 +5542,7 @@
       <c r="D26" s="74"/>
       <c r="E26" s="74"/>
     </row>
-    <row r="27" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="78" t="s">
         <v>51</v>
       </c>
@@ -5557,7 +5559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="79" t="s">
         <v>55</v>
       </c>
@@ -5571,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="79" t="s">
         <v>55</v>
       </c>
@@ -5585,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="79" t="s">
         <v>55</v>
       </c>
@@ -5599,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="79" t="s">
         <v>55</v>
       </c>
@@ -5695,8 +5697,8 @@
   </sheetPr>
   <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N31" activeCellId="0" sqref="N31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7846,7 +7848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
         <v>21</v>
       </c>
@@ -7885,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="68" t="s">
         <v>22</v>
       </c>
@@ -7924,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="68" t="s">
         <v>23</v>
       </c>
@@ -7963,7 +7965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="67" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="68" t="s">
         <v>67</v>
       </c>
@@ -7981,7 +7983,7 @@
       <c r="M8" s="72"/>
       <c r="N8" s="105"/>
     </row>
-    <row r="9" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="68" t="s">
         <v>25</v>
       </c>
@@ -8020,7 +8022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="68" t="s">
         <v>39</v>
       </c>
@@ -8057,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" s="67" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="106"/>
       <c r="B11" s="107"/>
       <c r="C11" s="108" t="s">
@@ -8079,7 +8081,7 @@
       <c r="M11" s="108"/>
       <c r="N11" s="108"/>
     </row>
-    <row r="12" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="75" t="s">
         <v>27</v>
       </c>
@@ -8109,7 +8111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="112" t="s">
         <v>41</v>
       </c>
@@ -8145,7 +8147,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="115"/>
       <c r="B14" s="116"/>
       <c r="C14" s="117" t="s">
@@ -8188,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="115"/>
       <c r="B15" s="116"/>
       <c r="C15" s="117" t="s">
@@ -8231,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="67" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="119"/>
       <c r="B16" s="120"/>
       <c r="C16" s="108" t="s">
@@ -8253,7 +8255,7 @@
       <c r="M16" s="108"/>
       <c r="N16" s="108"/>
     </row>
-    <row r="17" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="112" t="s">
         <v>47</v>
       </c>
@@ -8289,7 +8291,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="115"/>
       <c r="B18" s="116"/>
       <c r="C18" s="117" t="s">
@@ -8328,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" s="67" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="115"/>
       <c r="B19" s="116"/>
       <c r="C19" s="117" t="s">
@@ -8371,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" s="67" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="119"/>
       <c r="B20" s="120"/>
       <c r="C20" s="108" t="s">

</xml_diff>